<commit_message>
work to calibrate louisiana
</commit_message>
<xml_diff>
--- a/louisiana/transformations/templates/calibrated/louisiana/model_input_variables_louisiana_ce_calibrated.xlsx
+++ b/louisiana/transformations/templates/calibrated/louisiana/model_input_variables_louisiana_ce_calibrated.xlsx
@@ -13301,7 +13301,7 @@
         <v>146</v>
       </c>
       <c r="C100">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H100">
         <v>1</v>
@@ -13426,7 +13426,7 @@
         <v>147</v>
       </c>
       <c r="C101">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H101">
         <v>1</v>
@@ -13551,7 +13551,7 @@
         <v>148</v>
       </c>
       <c r="C102">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H102">
         <v>1</v>
@@ -13676,7 +13676,7 @@
         <v>149</v>
       </c>
       <c r="C103">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H103">
         <v>1</v>
@@ -13923,7 +13923,7 @@
         <v>151</v>
       </c>
       <c r="C105">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H105">
         <v>1</v>
@@ -14048,7 +14048,7 @@
         <v>152</v>
       </c>
       <c r="C106">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H106">
         <v>1</v>
@@ -17589,7 +17589,7 @@
         <v>181</v>
       </c>
       <c r="C135">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H135">
         <v>1</v>
@@ -18202,7 +18202,7 @@
         <v>186</v>
       </c>
       <c r="C140">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H140">
         <v>1</v>
@@ -18327,7 +18327,7 @@
         <v>187</v>
       </c>
       <c r="C141">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H141">
         <v>1</v>
@@ -18452,7 +18452,7 @@
         <v>188</v>
       </c>
       <c r="C142">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H142">
         <v>1</v>
@@ -18577,7 +18577,7 @@
         <v>189</v>
       </c>
       <c r="C143">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H143">
         <v>1</v>
@@ -18702,7 +18702,7 @@
         <v>190</v>
       </c>
       <c r="C144">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H144">
         <v>1</v>
@@ -18827,7 +18827,7 @@
         <v>191</v>
       </c>
       <c r="C145">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H145">
         <v>1</v>
@@ -18952,7 +18952,7 @@
         <v>192</v>
       </c>
       <c r="C146">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H146">
         <v>1</v>
@@ -26885,7 +26885,7 @@
         <v>257</v>
       </c>
       <c r="C211">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H211">
         <v>1</v>
@@ -27010,7 +27010,7 @@
         <v>258</v>
       </c>
       <c r="C212">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H212">
         <v>1</v>
@@ -27135,7 +27135,7 @@
         <v>259</v>
       </c>
       <c r="C213">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H213">
         <v>1</v>
@@ -27260,7 +27260,7 @@
         <v>260</v>
       </c>
       <c r="C214">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H214">
         <v>1</v>
@@ -28999,7 +28999,7 @@
         <v>146</v>
       </c>
       <c r="C2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -29124,7 +29124,7 @@
         <v>147</v>
       </c>
       <c r="C3">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -29249,7 +29249,7 @@
         <v>148</v>
       </c>
       <c r="C4">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -29374,7 +29374,7 @@
         <v>149</v>
       </c>
       <c r="C5">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -29499,7 +29499,7 @@
         <v>151</v>
       </c>
       <c r="C6">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -29624,7 +29624,7 @@
         <v>152</v>
       </c>
       <c r="C7">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -29871,7 +29871,7 @@
         <v>181</v>
       </c>
       <c r="C9">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -29996,7 +29996,7 @@
         <v>186</v>
       </c>
       <c r="C10">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -30121,7 +30121,7 @@
         <v>187</v>
       </c>
       <c r="C11">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -30246,7 +30246,7 @@
         <v>188</v>
       </c>
       <c r="C12">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -30371,7 +30371,7 @@
         <v>189</v>
       </c>
       <c r="C13">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -30496,7 +30496,7 @@
         <v>190</v>
       </c>
       <c r="C14">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -30621,7 +30621,7 @@
         <v>191</v>
       </c>
       <c r="C15">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -30746,7 +30746,7 @@
         <v>192</v>
       </c>
       <c r="C16">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -30993,7 +30993,7 @@
         <v>257</v>
       </c>
       <c r="C18">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -31118,7 +31118,7 @@
         <v>258</v>
       </c>
       <c r="C19">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -31243,7 +31243,7 @@
         <v>259</v>
       </c>
       <c r="C20">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -31368,7 +31368,7 @@
         <v>260</v>
       </c>
       <c r="C21">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -31643,7 +31643,7 @@
         <v>146</v>
       </c>
       <c r="C2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -31768,7 +31768,7 @@
         <v>147</v>
       </c>
       <c r="C3">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -31893,7 +31893,7 @@
         <v>148</v>
       </c>
       <c r="C4">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -32018,7 +32018,7 @@
         <v>149</v>
       </c>
       <c r="C5">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -32143,7 +32143,7 @@
         <v>151</v>
       </c>
       <c r="C6">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -32268,7 +32268,7 @@
         <v>152</v>
       </c>
       <c r="C7">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -32515,7 +32515,7 @@
         <v>181</v>
       </c>
       <c r="C9">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -32640,7 +32640,7 @@
         <v>186</v>
       </c>
       <c r="C10">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -32765,7 +32765,7 @@
         <v>187</v>
       </c>
       <c r="C11">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -32890,7 +32890,7 @@
         <v>188</v>
       </c>
       <c r="C12">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -33015,7 +33015,7 @@
         <v>189</v>
       </c>
       <c r="C13">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -33140,7 +33140,7 @@
         <v>190</v>
       </c>
       <c r="C14">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -33265,7 +33265,7 @@
         <v>191</v>
       </c>
       <c r="C15">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -33390,7 +33390,7 @@
         <v>192</v>
       </c>
       <c r="C16">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -33637,7 +33637,7 @@
         <v>257</v>
       </c>
       <c r="C18">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -33762,7 +33762,7 @@
         <v>258</v>
       </c>
       <c r="C19">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -33887,7 +33887,7 @@
         <v>259</v>
       </c>
       <c r="C20">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -34012,7 +34012,7 @@
         <v>260</v>
       </c>
       <c r="C21">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -34287,7 +34287,7 @@
         <v>146</v>
       </c>
       <c r="C2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -34412,7 +34412,7 @@
         <v>147</v>
       </c>
       <c r="C3">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -34537,7 +34537,7 @@
         <v>148</v>
       </c>
       <c r="C4">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -34662,7 +34662,7 @@
         <v>149</v>
       </c>
       <c r="C5">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -34787,7 +34787,7 @@
         <v>151</v>
       </c>
       <c r="C6">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -34912,7 +34912,7 @@
         <v>152</v>
       </c>
       <c r="C7">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -35159,7 +35159,7 @@
         <v>181</v>
       </c>
       <c r="C9">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -35284,7 +35284,7 @@
         <v>186</v>
       </c>
       <c r="C10">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -35409,7 +35409,7 @@
         <v>187</v>
       </c>
       <c r="C11">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -35534,7 +35534,7 @@
         <v>188</v>
       </c>
       <c r="C12">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -35659,7 +35659,7 @@
         <v>189</v>
       </c>
       <c r="C13">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -35784,7 +35784,7 @@
         <v>190</v>
       </c>
       <c r="C14">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -35909,7 +35909,7 @@
         <v>191</v>
       </c>
       <c r="C15">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -36034,7 +36034,7 @@
         <v>192</v>
       </c>
       <c r="C16">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -36281,7 +36281,7 @@
         <v>257</v>
       </c>
       <c r="C18">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -36406,7 +36406,7 @@
         <v>258</v>
       </c>
       <c r="C19">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -36531,7 +36531,7 @@
         <v>259</v>
       </c>
       <c r="C20">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -36656,7 +36656,7 @@
         <v>260</v>
       </c>
       <c r="C21">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -36931,7 +36931,7 @@
         <v>146</v>
       </c>
       <c r="C2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -37056,7 +37056,7 @@
         <v>147</v>
       </c>
       <c r="C3">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -37181,7 +37181,7 @@
         <v>148</v>
       </c>
       <c r="C4">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -37306,7 +37306,7 @@
         <v>149</v>
       </c>
       <c r="C5">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -37431,7 +37431,7 @@
         <v>151</v>
       </c>
       <c r="C6">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -37556,7 +37556,7 @@
         <v>152</v>
       </c>
       <c r="C7">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -37803,7 +37803,7 @@
         <v>181</v>
       </c>
       <c r="C9">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -37928,7 +37928,7 @@
         <v>186</v>
       </c>
       <c r="C10">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -38053,7 +38053,7 @@
         <v>187</v>
       </c>
       <c r="C11">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -38178,7 +38178,7 @@
         <v>188</v>
       </c>
       <c r="C12">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -38303,7 +38303,7 @@
         <v>189</v>
       </c>
       <c r="C13">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -38428,7 +38428,7 @@
         <v>190</v>
       </c>
       <c r="C14">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -38553,7 +38553,7 @@
         <v>191</v>
       </c>
       <c r="C15">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -38678,7 +38678,7 @@
         <v>192</v>
       </c>
       <c r="C16">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -38925,7 +38925,7 @@
         <v>257</v>
       </c>
       <c r="C18">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -39050,7 +39050,7 @@
         <v>258</v>
       </c>
       <c r="C19">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -39175,7 +39175,7 @@
         <v>259</v>
       </c>
       <c r="C20">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -39300,7 +39300,7 @@
         <v>260</v>
       </c>
       <c r="C21">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H21">
         <v>1</v>

</xml_diff>